<commit_message>
Successfully renamed EIN to UEI in one schema
The TODO file helps us remember everything we need to do.

We spent a substantial amount of time chasing the fact that the new UEI
type in the jsonnet schemas forced us to use "better" test data.
</commit_message>
<xml_diff>
--- a/backend/excel_templates/corrective-action-plan-template.xlsx
+++ b/backend/excel_templates/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="B0627566D24" lockStructure="1"/>
+  <workbookProtection workbookPassword="4EC0B4F9CC3" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <definedName name="reference_number">'Form'!$A$4:$A$3000</definedName>
     <definedName name="planned_action">'Form'!$C$4:$C$3000</definedName>
     <definedName name="contains_chart_or_table">'Form'!$G$4:$G$3000</definedName>
-    <definedName name="auditee_ein">'Form'!$B$2</definedName>
+    <definedName name="auditee_uei">'Form'!$B$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -15462,7 +15462,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="B0627566D24"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="4EC0B4F9CC3"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>
@@ -24461,7 +24461,7 @@
     <mergeCell ref="G111:H111"/>
     <mergeCell ref="A1615:B1615"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation sqref="A4:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A4), AND(LEN($A4) = 8, LEFT($A4, 2) = "20", ISNUMBER(MID($A4, 3, 2) * 1), MID($A4, 5, 1) = "-", ISNUMBER(RIGHT($A4, 3) * 1)))</formula1>
     </dataValidation>
@@ -24471,6 +24471,9 @@
     <dataValidation sqref="G4:G3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Y/N" error="Must be 'Y' or 'N'" type="list">
       <formula1>"Y,N"</formula1>
     </dataValidation>
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
+      <formula1>12</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
This adds some constants for UEIs
Which... need to be checked.
</commit_message>
<xml_diff>
--- a/backend/excel_templates/corrective-action-plan-template.xlsx
+++ b/backend/excel_templates/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="4EC0B4F9CC3" lockStructure="1"/>
+  <workbookProtection workbookPassword="429DA12093B" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -15462,7 +15462,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="4EC0B4F9CC3"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="429DA12093B"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>

</xml_diff>

<commit_message>
#940 Updated xlsx templates
</commit_message>
<xml_diff>
--- a/backend/excel_templates/corrective-action-plan-template.xlsx
+++ b/backend/excel_templates/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="429DA12093B" lockStructure="1"/>
+  <workbookProtection workbookPassword="423044D506B3" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -15462,7 +15462,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="429DA12093B"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="423044D506B3"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>

</xml_diff>

<commit_message>
#940 Regenerated xlsx templates
</commit_message>
<xml_diff>
--- a/backend/excel_templates/corrective-action-plan-template.xlsx
+++ b/backend/excel_templates/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="423044D506B3" lockStructure="1"/>
+  <workbookProtection workbookPassword="47D46116087" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -15462,7 +15462,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="423044D506B3"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="47D46116087"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>

</xml_diff>

<commit_message>
#940 Regenerated xlsx files
</commit_message>
<xml_diff>
--- a/backend/excel_templates/corrective-action-plan-template.xlsx
+++ b/backend/excel_templates/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="47D1243FC976" lockStructure="1"/>
+  <workbookProtection workbookPassword="10C2F1A42F932" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -30442,7 +30442,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="47D1243FC976"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10C2F1A42F932"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>

</xml_diff>